<commit_message>
bug fix with coal and iron
</commit_message>
<xml_diff>
--- a/sources/ТЗ.xlsx
+++ b/sources/ТЗ.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8633EE1-8829-394B-B531-0F8F1AC7E4D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA6BA2D8-5C23-4A2E-A407-F2CE1EB8C4B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2800" yWindow="500" windowWidth="31360" windowHeight="20460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="С гигачатом" sheetId="4" r:id="rId1"/>
@@ -731,7 +731,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="17">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1139,73 +1139,73 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1534,23 +1534,23 @@
   <dimension ref="A1:I138"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C68" sqref="C68"/>
+      <pane ySplit="1" topLeftCell="A81" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D95" sqref="D95"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.6640625" customWidth="1"/>
-    <col min="3" max="3" width="63.5" customWidth="1"/>
-    <col min="4" max="4" width="72.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.5" customWidth="1"/>
-    <col min="6" max="6" width="9.5" customWidth="1"/>
-    <col min="7" max="7" width="57.1640625" customWidth="1"/>
-    <col min="9" max="9" width="16.5" customWidth="1"/>
+    <col min="1" max="1" width="35.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" customWidth="1"/>
+    <col min="3" max="3" width="63.42578125" customWidth="1"/>
+    <col min="4" max="4" width="72.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" customWidth="1"/>
+    <col min="6" max="6" width="9.42578125" customWidth="1"/>
+    <col min="7" max="7" width="57.140625" customWidth="1"/>
+    <col min="9" max="9" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="32">
+    <row r="1" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
@@ -1579,7 +1579,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="32" customHeight="1">
+    <row r="2" spans="1:9" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="70" t="s">
         <v>35</v>
       </c>
@@ -1597,7 +1597,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="51">
+    <row r="3" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A3" s="70" t="s">
         <v>35</v>
       </c>
@@ -1615,7 +1615,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="51">
+    <row r="4" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A4" s="70" t="s">
         <v>35</v>
       </c>
@@ -1633,14 +1633,14 @@
         <v>169</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="16">
+    <row r="5" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="70"/>
       <c r="B5" s="56"/>
       <c r="C5" s="11"/>
       <c r="E5" s="11"/>
       <c r="G5" s="59"/>
     </row>
-    <row r="6" spans="1:9" ht="18" customHeight="1">
+    <row r="6" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="70" t="s">
         <v>35</v>
       </c>
@@ -1654,11 +1654,11 @@
         <v>27</v>
       </c>
       <c r="E6" s="11"/>
-      <c r="G6" s="93" t="s">
+      <c r="G6" s="75" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="51">
+    <row r="7" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A7" s="70" t="s">
         <v>35</v>
       </c>
@@ -1672,121 +1672,121 @@
         <v>27</v>
       </c>
       <c r="E7" s="11"/>
-      <c r="G7" s="93"/>
-    </row>
-    <row r="8" spans="1:9" ht="16">
+      <c r="G7" s="75"/>
+    </row>
+    <row r="8" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="70"/>
       <c r="B8" s="56"/>
       <c r="C8" s="9"/>
       <c r="D8" s="2"/>
       <c r="E8" s="11"/>
-      <c r="G8" s="93"/>
-    </row>
-    <row r="9" spans="1:9" ht="16">
+      <c r="G8" s="75"/>
+    </row>
+    <row r="9" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="70"/>
       <c r="B9" s="56"/>
       <c r="C9" s="9"/>
       <c r="D9" s="2"/>
       <c r="E9" s="11"/>
-      <c r="G9" s="93"/>
-    </row>
-    <row r="10" spans="1:9" ht="16">
+      <c r="G9" s="75"/>
+    </row>
+    <row r="10" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="70"/>
       <c r="B10" s="56"/>
       <c r="C10" s="9"/>
       <c r="D10" s="2"/>
       <c r="E10" s="11"/>
-      <c r="G10" s="93"/>
-    </row>
-    <row r="11" spans="1:9" ht="16">
+      <c r="G10" s="75"/>
+    </row>
+    <row r="11" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="70"/>
       <c r="B11" s="56"/>
       <c r="C11" s="9"/>
       <c r="D11" s="2"/>
       <c r="E11" s="11"/>
-      <c r="G11" s="93"/>
-    </row>
-    <row r="12" spans="1:9" ht="16">
+      <c r="G11" s="75"/>
+    </row>
+    <row r="12" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="70"/>
       <c r="B12" s="56"/>
       <c r="C12" s="9"/>
       <c r="D12" s="2"/>
       <c r="E12" s="11"/>
-      <c r="G12" s="93"/>
-    </row>
-    <row r="13" spans="1:9" ht="16">
+      <c r="G12" s="75"/>
+    </row>
+    <row r="13" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="70"/>
       <c r="B13" s="56"/>
       <c r="C13" s="9"/>
       <c r="D13" s="2"/>
       <c r="E13" s="11"/>
-      <c r="G13" s="93"/>
-    </row>
-    <row r="14" spans="1:9" ht="16">
+      <c r="G13" s="75"/>
+    </row>
+    <row r="14" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="70"/>
       <c r="B14" s="56"/>
       <c r="C14" s="9"/>
       <c r="D14" s="2"/>
       <c r="E14" s="11"/>
-      <c r="G14" s="93"/>
-    </row>
-    <row r="15" spans="1:9" ht="16">
+      <c r="G14" s="75"/>
+    </row>
+    <row r="15" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="70"/>
       <c r="B15" s="56"/>
       <c r="C15" s="9"/>
       <c r="D15" s="2"/>
       <c r="E15" s="11"/>
-      <c r="G15" s="93"/>
-    </row>
-    <row r="16" spans="1:9" ht="16">
+      <c r="G15" s="75"/>
+    </row>
+    <row r="16" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="70"/>
       <c r="B16" s="56"/>
       <c r="C16" s="9"/>
       <c r="D16" s="2"/>
       <c r="E16" s="11"/>
-      <c r="G16" s="93"/>
-    </row>
-    <row r="17" spans="1:9" ht="16">
+      <c r="G16" s="75"/>
+    </row>
+    <row r="17" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="70"/>
       <c r="B17" s="56"/>
       <c r="C17" s="9"/>
       <c r="D17" s="2"/>
       <c r="E17" s="11"/>
-      <c r="G17" s="93"/>
-    </row>
-    <row r="18" spans="1:9" ht="16">
+      <c r="G17" s="75"/>
+    </row>
+    <row r="18" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="70"/>
       <c r="B18" s="56"/>
       <c r="C18" s="9"/>
       <c r="D18" s="2"/>
       <c r="E18" s="11"/>
-      <c r="G18" s="93"/>
-    </row>
-    <row r="19" spans="1:9" ht="16">
+      <c r="G18" s="75"/>
+    </row>
+    <row r="19" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="70"/>
       <c r="B19" s="56"/>
       <c r="C19" s="9"/>
       <c r="D19" s="2"/>
       <c r="E19" s="11"/>
-      <c r="G19" s="93"/>
-    </row>
-    <row r="20" spans="1:9" ht="16">
+      <c r="G19" s="75"/>
+    </row>
+    <row r="20" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="70"/>
       <c r="B20" s="56"/>
       <c r="C20" s="9"/>
       <c r="D20" s="2"/>
       <c r="E20" s="11"/>
-      <c r="G20" s="93"/>
-    </row>
-    <row r="21" spans="1:9" ht="16">
+      <c r="G20" s="75"/>
+    </row>
+    <row r="21" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="70"/>
       <c r="B21" s="56"/>
       <c r="C21" s="10"/>
       <c r="D21" s="2"/>
       <c r="E21" s="11"/>
-      <c r="G21" s="93"/>
-    </row>
-    <row r="22" spans="1:9" ht="16">
+      <c r="G21" s="75"/>
+    </row>
+    <row r="22" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="70"/>
       <c r="B22" s="56"/>
       <c r="C22" s="11"/>
@@ -1794,7 +1794,7 @@
       <c r="E22" s="11"/>
       <c r="G22" s="59"/>
     </row>
-    <row r="23" spans="1:9" ht="17.5" customHeight="1">
+    <row r="23" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="70" t="s">
         <v>35</v>
       </c>
@@ -1808,11 +1808,11 @@
         <v>26</v>
       </c>
       <c r="E23" s="11"/>
-      <c r="G23" s="93" t="s">
+      <c r="G23" s="75" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="51">
+    <row r="24" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A24" s="70" t="s">
         <v>35</v>
       </c>
@@ -1826,41 +1826,41 @@
         <v>26</v>
       </c>
       <c r="E24" s="11"/>
-      <c r="G24" s="93"/>
-    </row>
-    <row r="25" spans="1:9" ht="16">
+      <c r="G24" s="75"/>
+    </row>
+    <row r="25" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="70"/>
       <c r="B25" s="56"/>
       <c r="C25" s="15"/>
       <c r="D25" s="2"/>
       <c r="E25" s="11"/>
-      <c r="G25" s="93"/>
-    </row>
-    <row r="26" spans="1:9" ht="16">
+      <c r="G25" s="75"/>
+    </row>
+    <row r="26" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="70"/>
       <c r="B26" s="56"/>
       <c r="C26" s="15"/>
       <c r="D26" s="2"/>
       <c r="E26" s="11"/>
-      <c r="G26" s="93"/>
-    </row>
-    <row r="27" spans="1:9" ht="16">
+      <c r="G26" s="75"/>
+    </row>
+    <row r="27" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="70"/>
       <c r="B27" s="56"/>
       <c r="C27" s="15"/>
       <c r="D27" s="2"/>
       <c r="E27" s="11"/>
-      <c r="G27" s="93"/>
-    </row>
-    <row r="28" spans="1:9" ht="16">
+      <c r="G27" s="75"/>
+    </row>
+    <row r="28" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="70"/>
       <c r="B28" s="56"/>
       <c r="C28" s="16"/>
       <c r="D28" s="2"/>
       <c r="E28" s="11"/>
-      <c r="G28" s="93"/>
-    </row>
-    <row r="29" spans="1:9" ht="51">
+      <c r="G28" s="75"/>
+    </row>
+    <row r="29" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A29" s="70" t="s">
         <v>35</v>
       </c>
@@ -1873,7 +1873,7 @@
       <c r="F29" s="29"/>
       <c r="G29" s="29"/>
     </row>
-    <row r="30" spans="1:9" ht="51">
+    <row r="30" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A30" s="70" t="s">
         <v>35</v>
       </c>
@@ -1888,7 +1888,7 @@
       <c r="H30" s="23"/>
       <c r="I30" s="23"/>
     </row>
-    <row r="31" spans="1:9" ht="16" customHeight="1">
+    <row r="31" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="71" t="s">
         <v>41</v>
       </c>
@@ -1898,7 +1898,7 @@
       <c r="C31" s="24"/>
       <c r="D31" s="24"/>
     </row>
-    <row r="32" spans="1:9" ht="30" customHeight="1">
+    <row r="32" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="71" t="s">
         <v>41</v>
       </c>
@@ -1915,61 +1915,61 @@
         <v>173</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="16">
+    <row r="33" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="71"/>
       <c r="B33" s="57"/>
       <c r="C33" s="4"/>
       <c r="D33" s="2"/>
     </row>
-    <row r="34" spans="1:9" ht="16">
+    <row r="34" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="71"/>
       <c r="B34" s="57"/>
       <c r="C34" s="5"/>
       <c r="D34" s="2"/>
     </row>
-    <row r="35" spans="1:9" ht="16">
+    <row r="35" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="71"/>
       <c r="B35" s="57"/>
       <c r="C35" s="5"/>
       <c r="D35" s="2"/>
     </row>
-    <row r="36" spans="1:9" ht="16">
+    <row r="36" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="71"/>
       <c r="B36" s="57"/>
       <c r="C36" s="5"/>
       <c r="D36" s="2"/>
     </row>
-    <row r="37" spans="1:9" ht="16">
+    <row r="37" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="71"/>
       <c r="B37" s="57"/>
       <c r="C37" s="5"/>
       <c r="D37" s="2"/>
     </row>
-    <row r="38" spans="1:9" ht="16">
+    <row r="38" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="71"/>
       <c r="B38" s="57"/>
       <c r="C38" s="5"/>
       <c r="D38" s="2"/>
     </row>
-    <row r="39" spans="1:9" ht="16">
+    <row r="39" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="71"/>
       <c r="B39" s="57"/>
       <c r="C39" s="5"/>
       <c r="D39" s="2"/>
     </row>
-    <row r="40" spans="1:9" ht="16">
+    <row r="40" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="71"/>
       <c r="B40" s="57"/>
       <c r="C40" s="5"/>
       <c r="D40" s="2"/>
     </row>
-    <row r="41" spans="1:9" ht="16">
+    <row r="41" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="71"/>
       <c r="B41" s="57"/>
       <c r="C41" s="6"/>
       <c r="D41" s="2"/>
     </row>
-    <row r="42" spans="1:9" ht="34">
+    <row r="42" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A42" s="71" t="s">
         <v>41</v>
       </c>
@@ -1982,7 +1982,7 @@
       <c r="F42" s="29"/>
       <c r="G42" s="29"/>
     </row>
-    <row r="43" spans="1:9" ht="34">
+    <row r="43" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A43" s="71" t="s">
         <v>41</v>
       </c>
@@ -1997,7 +1997,7 @@
       <c r="H43" s="23"/>
       <c r="I43" s="23"/>
     </row>
-    <row r="44" spans="1:9" ht="15" customHeight="1">
+    <row r="44" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="72" t="s">
         <v>68</v>
       </c>
@@ -2005,7 +2005,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="45" spans="1:9" ht="15.5" customHeight="1">
+    <row r="45" spans="1:9" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="72" t="s">
         <v>68</v>
       </c>
@@ -2016,7 +2016,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="46" spans="1:9" ht="34">
+    <row r="46" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A46" s="72" t="s">
         <v>68</v>
       </c>
@@ -2036,7 +2036,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="47" spans="1:9" ht="34">
+    <row r="47" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A47" s="72" t="s">
         <v>68</v>
       </c>
@@ -2053,7 +2053,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="48" spans="1:9" ht="34">
+    <row r="48" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A48" s="72" t="s">
         <v>68</v>
       </c>
@@ -2072,7 +2072,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="49" spans="1:9" ht="34">
+    <row r="49" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A49" s="72" t="s">
         <v>68</v>
       </c>
@@ -2090,7 +2090,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="50" spans="1:9" ht="34">
+    <row r="50" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A50" s="72" t="s">
         <v>68</v>
       </c>
@@ -2109,7 +2109,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="51" spans="1:9" ht="48">
+    <row r="51" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A51" s="72" t="s">
         <v>68</v>
       </c>
@@ -2127,7 +2127,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="52" spans="1:9" ht="34">
+    <row r="52" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A52" s="72" t="s">
         <v>68</v>
       </c>
@@ -2140,7 +2140,7 @@
       <c r="F52" s="29"/>
       <c r="G52" s="29"/>
     </row>
-    <row r="53" spans="1:9" ht="34">
+    <row r="53" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A53" s="72" t="s">
         <v>68</v>
       </c>
@@ -2155,7 +2155,7 @@
       <c r="H53" s="23"/>
       <c r="I53" s="23"/>
     </row>
-    <row r="54" spans="1:9" ht="14.5" customHeight="1">
+    <row r="54" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="57" t="s">
         <v>69</v>
       </c>
@@ -2163,7 +2163,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="55" spans="1:9" ht="16">
+    <row r="55" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A55" s="57" t="s">
         <v>69</v>
       </c>
@@ -2176,7 +2176,7 @@
       <c r="D55" s="7"/>
       <c r="E55" s="7"/>
     </row>
-    <row r="56" spans="1:9" ht="64">
+    <row r="56" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A56" s="57" t="s">
         <v>69</v>
       </c>
@@ -2193,7 +2193,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="57" spans="1:9" ht="32">
+    <row r="57" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A57" s="57" t="s">
         <v>69</v>
       </c>
@@ -2210,7 +2210,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="58" spans="1:9" ht="32">
+    <row r="58" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A58" s="57"/>
       <c r="B58" s="57"/>
       <c r="C58" s="37"/>
@@ -2220,7 +2220,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="59" spans="1:9" ht="32">
+    <row r="59" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A59" s="57"/>
       <c r="B59" s="57"/>
       <c r="C59" s="37"/>
@@ -2230,7 +2230,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="60" spans="1:9" ht="32">
+    <row r="60" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A60" s="57"/>
       <c r="B60" s="57"/>
       <c r="C60" s="37"/>
@@ -2240,7 +2240,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="61" spans="1:9" ht="32">
+    <row r="61" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A61" s="57"/>
       <c r="B61" s="57"/>
       <c r="C61" s="37"/>
@@ -2250,7 +2250,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="62" spans="1:9" ht="32">
+    <row r="62" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A62" s="57"/>
       <c r="B62" s="57"/>
       <c r="C62" s="37"/>
@@ -2260,7 +2260,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="63" spans="1:9" ht="32">
+    <row r="63" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A63" s="57"/>
       <c r="B63" s="57"/>
       <c r="C63" s="37"/>
@@ -2270,7 +2270,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="64" spans="1:9" ht="32">
+    <row r="64" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A64" s="57"/>
       <c r="B64" s="57"/>
       <c r="C64" s="37"/>
@@ -2280,7 +2280,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="65" spans="1:9" ht="32">
+    <row r="65" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A65" s="57"/>
       <c r="B65" s="57"/>
       <c r="C65" s="37"/>
@@ -2290,7 +2290,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="66" spans="1:9" ht="32">
+    <row r="66" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A66" s="57"/>
       <c r="B66" s="57"/>
       <c r="C66" s="37"/>
@@ -2300,7 +2300,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="67" spans="1:9" ht="104" customHeight="1">
+    <row r="67" spans="1:9" ht="104.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="57" t="s">
         <v>69</v>
       </c>
@@ -2319,7 +2319,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="68" spans="1:9" ht="32">
+    <row r="68" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A68" s="57" t="s">
         <v>69</v>
       </c>
@@ -2337,7 +2337,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="69" spans="1:9" ht="32">
+    <row r="69" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A69" s="57" t="s">
         <v>69</v>
       </c>
@@ -2353,7 +2353,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="70" spans="1:9" ht="32">
+    <row r="70" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A70" s="57" t="s">
         <v>69</v>
       </c>
@@ -2371,7 +2371,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="71" spans="1:9" ht="16">
+    <row r="71" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A71" s="57" t="s">
         <v>69</v>
       </c>
@@ -2386,36 +2386,36 @@
       <c r="H71" s="23"/>
       <c r="I71" s="23"/>
     </row>
-    <row r="72" spans="1:9" ht="15.5" customHeight="1">
-      <c r="A72" s="83" t="s">
+    <row r="72" spans="1:9" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="84" t="s">
         <v>109</v>
       </c>
-      <c r="B72" s="91" t="s">
+      <c r="B72" s="80" t="s">
         <v>70</v>
       </c>
-      <c r="C72" s="75" t="s">
+      <c r="C72" s="76" t="s">
         <v>110</v>
       </c>
-      <c r="D72" s="94" t="s">
+      <c r="D72" s="78" t="s">
         <v>72</v>
       </c>
-      <c r="E72" s="96"/>
-      <c r="F72" s="91"/>
-      <c r="G72" s="93" t="s">
+      <c r="E72" s="82"/>
+      <c r="F72" s="80"/>
+      <c r="G72" s="75" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="73" spans="1:9" ht="44.5" customHeight="1">
-      <c r="A73" s="90"/>
-      <c r="B73" s="92"/>
-      <c r="C73" s="76"/>
-      <c r="D73" s="95"/>
-      <c r="E73" s="97"/>
-      <c r="F73" s="92"/>
-      <c r="G73" s="93"/>
-    </row>
-    <row r="74" spans="1:9" ht="16">
-      <c r="A74" s="84"/>
+    <row r="73" spans="1:9" ht="44.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="86"/>
+      <c r="B73" s="81"/>
+      <c r="C73" s="77"/>
+      <c r="D73" s="79"/>
+      <c r="E73" s="83"/>
+      <c r="F73" s="81"/>
+      <c r="G73" s="75"/>
+    </row>
+    <row r="74" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A74" s="85"/>
       <c r="B74" s="27" t="s">
         <v>111</v>
       </c>
@@ -2427,8 +2427,8 @@
       <c r="H74" s="23"/>
       <c r="I74" s="23"/>
     </row>
-    <row r="75" spans="1:9" ht="16">
-      <c r="A75" s="83" t="s">
+    <row r="75" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A75" s="84" t="s">
         <v>73</v>
       </c>
       <c r="B75" s="24" t="s">
@@ -2444,8 +2444,8 @@
         <v>188</v>
       </c>
     </row>
-    <row r="76" spans="1:9" ht="16">
-      <c r="A76" s="84"/>
+    <row r="76" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A76" s="85"/>
       <c r="B76" s="27" t="s">
         <v>111</v>
       </c>
@@ -2457,8 +2457,8 @@
       <c r="H76" s="23"/>
       <c r="I76" s="23"/>
     </row>
-    <row r="77" spans="1:9" ht="16">
-      <c r="A77" s="83" t="s">
+    <row r="77" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A77" s="84" t="s">
         <v>75</v>
       </c>
       <c r="B77" s="24" t="s">
@@ -2475,8 +2475,8 @@
         <v>188</v>
       </c>
     </row>
-    <row r="78" spans="1:9" ht="16">
-      <c r="A78" s="84"/>
+    <row r="78" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A78" s="85"/>
       <c r="B78" s="27" t="s">
         <v>111</v>
       </c>
@@ -2488,8 +2488,8 @@
       <c r="H78" s="23"/>
       <c r="I78" s="23"/>
     </row>
-    <row r="79" spans="1:9" ht="16">
-      <c r="A79" s="83" t="s">
+    <row r="79" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A79" s="84" t="s">
         <v>77</v>
       </c>
       <c r="B79" s="24" t="s">
@@ -2506,8 +2506,8 @@
         <v>188</v>
       </c>
     </row>
-    <row r="80" spans="1:9" ht="16">
-      <c r="A80" s="84"/>
+    <row r="80" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A80" s="85"/>
       <c r="B80" s="27" t="s">
         <v>111</v>
       </c>
@@ -2519,8 +2519,8 @@
       <c r="H80" s="23"/>
       <c r="I80" s="23"/>
     </row>
-    <row r="81" spans="1:9" ht="16">
-      <c r="A81" s="83" t="s">
+    <row r="81" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A81" s="84" t="s">
         <v>79</v>
       </c>
       <c r="B81" s="24" t="s">
@@ -2537,8 +2537,8 @@
         <v>188</v>
       </c>
     </row>
-    <row r="82" spans="1:9" ht="16">
-      <c r="A82" s="84"/>
+    <row r="82" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A82" s="85"/>
       <c r="B82" s="27" t="s">
         <v>111</v>
       </c>
@@ -2550,8 +2550,8 @@
       <c r="H82" s="23"/>
       <c r="I82" s="23"/>
     </row>
-    <row r="83" spans="1:9" ht="16">
-      <c r="A83" s="83" t="s">
+    <row r="83" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A83" s="84" t="s">
         <v>81</v>
       </c>
       <c r="B83" s="24" t="s">
@@ -2568,8 +2568,8 @@
         <v>188</v>
       </c>
     </row>
-    <row r="84" spans="1:9" ht="16">
-      <c r="A84" s="84"/>
+    <row r="84" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A84" s="85"/>
       <c r="B84" s="27" t="s">
         <v>111</v>
       </c>
@@ -2581,8 +2581,8 @@
       <c r="H84" s="23"/>
       <c r="I84" s="23"/>
     </row>
-    <row r="85" spans="1:9" ht="16">
-      <c r="A85" s="83" t="s">
+    <row r="85" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A85" s="84" t="s">
         <v>83</v>
       </c>
       <c r="B85" s="24" t="s">
@@ -2599,8 +2599,8 @@
         <v>188</v>
       </c>
     </row>
-    <row r="86" spans="1:9" ht="16">
-      <c r="A86" s="84"/>
+    <row r="86" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A86" s="85"/>
       <c r="B86" s="27" t="s">
         <v>111</v>
       </c>
@@ -2612,8 +2612,8 @@
       <c r="H86" s="23"/>
       <c r="I86" s="23"/>
     </row>
-    <row r="87" spans="1:9" ht="16">
-      <c r="A87" s="83" t="s">
+    <row r="87" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A87" s="84" t="s">
         <v>85</v>
       </c>
       <c r="B87" s="24" t="s">
@@ -2630,8 +2630,8 @@
         <v>188</v>
       </c>
     </row>
-    <row r="88" spans="1:9" ht="16">
-      <c r="A88" s="84"/>
+    <row r="88" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A88" s="85"/>
       <c r="B88" s="27" t="s">
         <v>111</v>
       </c>
@@ -2643,8 +2643,8 @@
       <c r="H88" s="23"/>
       <c r="I88" s="23"/>
     </row>
-    <row r="89" spans="1:9" ht="16">
-      <c r="A89" s="83" t="s">
+    <row r="89" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A89" s="84" t="s">
         <v>87</v>
       </c>
       <c r="B89" s="24" t="s">
@@ -2661,8 +2661,8 @@
         <v>188</v>
       </c>
     </row>
-    <row r="90" spans="1:9" ht="16">
-      <c r="A90" s="84"/>
+    <row r="90" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A90" s="85"/>
       <c r="B90" s="27" t="s">
         <v>111</v>
       </c>
@@ -2674,8 +2674,8 @@
       <c r="H90" s="23"/>
       <c r="I90" s="23"/>
     </row>
-    <row r="91" spans="1:9" ht="16">
-      <c r="A91" s="83" t="s">
+    <row r="91" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A91" s="84" t="s">
         <v>89</v>
       </c>
       <c r="B91" s="24" t="s">
@@ -2692,8 +2692,8 @@
         <v>188</v>
       </c>
     </row>
-    <row r="92" spans="1:9" ht="16">
-      <c r="A92" s="84"/>
+    <row r="92" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A92" s="85"/>
       <c r="B92" s="27" t="s">
         <v>111</v>
       </c>
@@ -2705,8 +2705,8 @@
       <c r="H92" s="23"/>
       <c r="I92" s="23"/>
     </row>
-    <row r="93" spans="1:9" ht="16">
-      <c r="A93" s="83" t="s">
+    <row r="93" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A93" s="84" t="s">
         <v>91</v>
       </c>
       <c r="B93" s="24" t="s">
@@ -2723,8 +2723,8 @@
         <v>188</v>
       </c>
     </row>
-    <row r="94" spans="1:9" ht="16">
-      <c r="A94" s="84"/>
+    <row r="94" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A94" s="85"/>
       <c r="B94" s="27" t="s">
         <v>111</v>
       </c>
@@ -2736,8 +2736,8 @@
       <c r="H94" s="23"/>
       <c r="I94" s="23"/>
     </row>
-    <row r="95" spans="1:9" ht="32">
-      <c r="A95" s="85" t="s">
+    <row r="95" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A95" s="90" t="s">
         <v>112</v>
       </c>
       <c r="B95" s="24" t="s">
@@ -2747,15 +2747,15 @@
         <v>110</v>
       </c>
       <c r="D95" s="44" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="E95" s="41"/>
       <c r="G95" s="59" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="96" spans="1:9" ht="16">
-      <c r="A96" s="84"/>
+    <row r="96" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A96" s="85"/>
       <c r="B96" s="27" t="s">
         <v>111</v>
       </c>
@@ -2767,8 +2767,8 @@
       <c r="H96" s="23"/>
       <c r="I96" s="23"/>
     </row>
-    <row r="97" spans="1:9" ht="16">
-      <c r="A97" s="86" t="s">
+    <row r="97" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A97" s="91" t="s">
         <v>113</v>
       </c>
       <c r="B97" s="24" t="s">
@@ -2778,28 +2778,27 @@
         <v>110</v>
       </c>
       <c r="D97" s="44" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E97" s="41"/>
       <c r="G97" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="98" spans="1:9" ht="16">
-      <c r="A98" s="79"/>
+    <row r="98" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A98" s="92"/>
       <c r="B98" s="27" t="s">
         <v>111</v>
       </c>
       <c r="C98" s="23"/>
-      <c r="D98" s="23"/>
       <c r="E98" s="23"/>
       <c r="F98" s="23"/>
       <c r="G98" s="23"/>
       <c r="H98" s="23"/>
       <c r="I98" s="23"/>
     </row>
-    <row r="99" spans="1:9" ht="16">
-      <c r="A99" s="83" t="s">
+    <row r="99" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A99" s="84" t="s">
         <v>114</v>
       </c>
       <c r="B99" s="24" t="s">
@@ -2816,8 +2815,8 @@
         <v>189</v>
       </c>
     </row>
-    <row r="100" spans="1:9" ht="16">
-      <c r="A100" s="84"/>
+    <row r="100" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A100" s="85"/>
       <c r="B100" s="27" t="s">
         <v>111</v>
       </c>
@@ -2829,19 +2828,19 @@
       <c r="H100" s="23"/>
       <c r="I100" s="23"/>
     </row>
-    <row r="101" spans="1:9" ht="16">
-      <c r="A101" s="87" t="s">
+    <row r="101" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A101" s="93" t="s">
         <v>115</v>
       </c>
-      <c r="B101" s="75" t="s">
+      <c r="B101" s="76" t="s">
         <v>70</v>
       </c>
       <c r="C101" s="7"/>
       <c r="D101" s="7"/>
     </row>
-    <row r="102" spans="1:9" ht="16">
-      <c r="A102" s="88"/>
-      <c r="B102" s="76"/>
+    <row r="102" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A102" s="94"/>
+      <c r="B102" s="77"/>
       <c r="C102" s="7" t="s">
         <v>116</v>
       </c>
@@ -2850,8 +2849,8 @@
       </c>
       <c r="F102" s="35"/>
     </row>
-    <row r="103" spans="1:9" ht="16">
-      <c r="A103" s="88"/>
+    <row r="103" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A103" s="94"/>
       <c r="B103" s="7" t="s">
         <v>118</v>
       </c>
@@ -2865,8 +2864,8 @@
         <v>182</v>
       </c>
     </row>
-    <row r="104" spans="1:9" ht="16">
-      <c r="A104" s="89"/>
+    <row r="104" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A104" s="95"/>
       <c r="B104" s="27" t="s">
         <v>31</v>
       </c>
@@ -2878,8 +2877,8 @@
       <c r="H104" s="23"/>
       <c r="I104" s="23"/>
     </row>
-    <row r="105" spans="1:9" ht="16">
-      <c r="A105" s="77" t="s">
+    <row r="105" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A105" s="96" t="s">
         <v>121</v>
       </c>
       <c r="B105" s="65" t="s">
@@ -2897,8 +2896,8 @@
       <c r="H105" s="41"/>
       <c r="I105" s="41"/>
     </row>
-    <row r="106" spans="1:9" ht="16">
-      <c r="A106" s="78"/>
+    <row r="106" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A106" s="97"/>
       <c r="B106" s="39" t="s">
         <v>118</v>
       </c>
@@ -2912,8 +2911,8 @@
         <v>158</v>
       </c>
     </row>
-    <row r="107" spans="1:9" ht="16">
-      <c r="A107" s="79"/>
+    <row r="107" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A107" s="92"/>
       <c r="B107" s="49" t="s">
         <v>31</v>
       </c>
@@ -2924,8 +2923,8 @@
       <c r="H107" s="23"/>
       <c r="I107" s="23"/>
     </row>
-    <row r="108" spans="1:9" ht="16">
-      <c r="A108" s="77" t="s">
+    <row r="108" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A108" s="96" t="s">
         <v>124</v>
       </c>
       <c r="B108" s="65" t="s">
@@ -2943,8 +2942,8 @@
       <c r="H108" s="41"/>
       <c r="I108" s="41"/>
     </row>
-    <row r="109" spans="1:9" ht="16">
-      <c r="A109" s="78"/>
+    <row r="109" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A109" s="97"/>
       <c r="B109" s="39" t="s">
         <v>118</v>
       </c>
@@ -2958,8 +2957,8 @@
         <v>183</v>
       </c>
     </row>
-    <row r="110" spans="1:9" ht="16">
-      <c r="A110" s="79"/>
+    <row r="110" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A110" s="92"/>
       <c r="B110" s="49" t="s">
         <v>31</v>
       </c>
@@ -2971,8 +2970,8 @@
       <c r="H110" s="23"/>
       <c r="I110" s="23"/>
     </row>
-    <row r="111" spans="1:9" ht="16">
-      <c r="A111" s="77" t="s">
+    <row r="111" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A111" s="96" t="s">
         <v>127</v>
       </c>
       <c r="B111" s="65" t="s">
@@ -2990,8 +2989,8 @@
       <c r="H111" s="41"/>
       <c r="I111" s="41"/>
     </row>
-    <row r="112" spans="1:9" ht="16">
-      <c r="A112" s="78"/>
+    <row r="112" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A112" s="97"/>
       <c r="B112" s="39" t="s">
         <v>118</v>
       </c>
@@ -3005,8 +3004,8 @@
         <v>184</v>
       </c>
     </row>
-    <row r="113" spans="1:9" ht="16">
-      <c r="A113" s="79"/>
+    <row r="113" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A113" s="92"/>
       <c r="B113" s="49" t="s">
         <v>31</v>
       </c>
@@ -3017,8 +3016,8 @@
       <c r="H113" s="23"/>
       <c r="I113" s="23"/>
     </row>
-    <row r="114" spans="1:9" ht="16">
-      <c r="A114" s="77" t="s">
+    <row r="114" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A114" s="96" t="s">
         <v>130</v>
       </c>
       <c r="B114" s="65" t="s">
@@ -3036,8 +3035,8 @@
       <c r="H114" s="41"/>
       <c r="I114" s="41"/>
     </row>
-    <row r="115" spans="1:9" ht="16">
-      <c r="A115" s="78"/>
+    <row r="115" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A115" s="97"/>
       <c r="B115" s="39" t="s">
         <v>118</v>
       </c>
@@ -3051,8 +3050,8 @@
         <v>185</v>
       </c>
     </row>
-    <row r="116" spans="1:9" ht="16">
-      <c r="A116" s="79"/>
+    <row r="116" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A116" s="92"/>
       <c r="B116" s="49" t="s">
         <v>31</v>
       </c>
@@ -3063,8 +3062,8 @@
       <c r="H116" s="23"/>
       <c r="I116" s="23"/>
     </row>
-    <row r="117" spans="1:9" ht="16">
-      <c r="A117" s="80" t="s">
+    <row r="117" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A117" s="87" t="s">
         <v>133</v>
       </c>
       <c r="B117" s="65" t="s">
@@ -3082,8 +3081,8 @@
       <c r="H117" s="41"/>
       <c r="I117" s="41"/>
     </row>
-    <row r="118" spans="1:9" ht="16">
-      <c r="A118" s="81"/>
+    <row r="118" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A118" s="88"/>
       <c r="B118" s="39" t="s">
         <v>118</v>
       </c>
@@ -3097,8 +3096,8 @@
         <v>186</v>
       </c>
     </row>
-    <row r="119" spans="1:9" ht="16">
-      <c r="A119" s="82"/>
+    <row r="119" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A119" s="89"/>
       <c r="B119" s="49" t="s">
         <v>31</v>
       </c>
@@ -3109,7 +3108,7 @@
       <c r="H119" s="23"/>
       <c r="I119" s="23"/>
     </row>
-    <row r="120" spans="1:9" ht="16">
+    <row r="120" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A120" s="45" t="s">
         <v>137</v>
       </c>
@@ -3117,7 +3116,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="121" spans="1:9" ht="16">
+    <row r="121" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A121" s="45" t="s">
         <v>138</v>
       </c>
@@ -3125,7 +3124,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="122" spans="1:9" ht="16">
+    <row r="122" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A122" s="45" t="s">
         <v>139</v>
       </c>
@@ -3133,7 +3132,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="123" spans="1:9" ht="16">
+    <row r="123" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A123" s="47" t="s">
         <v>140</v>
       </c>
@@ -3141,7 +3140,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="124" spans="1:9" ht="16">
+    <row r="124" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A124" s="47" t="s">
         <v>141</v>
       </c>
@@ -3149,7 +3148,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="125" spans="1:9" ht="16">
+    <row r="125" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A125" s="47" t="s">
         <v>142</v>
       </c>
@@ -3157,7 +3156,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="126" spans="1:9" ht="16">
+    <row r="126" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A126" s="47" t="s">
         <v>143</v>
       </c>
@@ -3165,7 +3164,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="127" spans="1:9" ht="16">
+    <row r="127" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A127" s="47" t="s">
         <v>144</v>
       </c>
@@ -3173,7 +3172,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="128" spans="1:9" ht="16">
+    <row r="128" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A128" s="47" t="s">
         <v>145</v>
       </c>
@@ -3181,7 +3180,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="129" spans="1:6" ht="16">
+    <row r="129" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A129" s="47" t="s">
         <v>146</v>
       </c>
@@ -3189,7 +3188,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="130" spans="1:6" ht="16">
+    <row r="130" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A130" s="47" t="s">
         <v>147</v>
       </c>
@@ -3197,7 +3196,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="131" spans="1:6" ht="16">
+    <row r="131" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A131" s="47" t="s">
         <v>148</v>
       </c>
@@ -3205,7 +3204,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="132" spans="1:6" ht="16">
+    <row r="132" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A132" s="47" t="s">
         <v>149</v>
       </c>
@@ -3213,7 +3212,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="133" spans="1:6" ht="16">
+    <row r="133" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A133" s="47" t="s">
         <v>150</v>
       </c>
@@ -3221,7 +3220,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="134" spans="1:6" ht="16">
+    <row r="134" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A134" s="47" t="s">
         <v>151</v>
       </c>
@@ -3229,7 +3228,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="135" spans="1:6" ht="16">
+    <row r="135" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A135" s="47" t="s">
         <v>152</v>
       </c>
@@ -3237,7 +3236,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="136" spans="1:6" ht="16">
+    <row r="136" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A136" s="47" t="s">
         <v>153</v>
       </c>
@@ -3245,7 +3244,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="137" spans="1:6" ht="16">
+    <row r="137" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A137" s="47" t="s">
         <v>154</v>
       </c>
@@ -3253,7 +3252,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="138" spans="1:6" ht="16">
+    <row r="138" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A138" s="48" t="s">
         <v>155</v>
       </c>
@@ -3268,13 +3267,18 @@
   </sheetData>
   <autoFilter ref="A23:G138" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <mergeCells count="29">
-    <mergeCell ref="G6:G21"/>
-    <mergeCell ref="G23:G28"/>
-    <mergeCell ref="C72:C73"/>
-    <mergeCell ref="D72:D73"/>
-    <mergeCell ref="G72:G73"/>
-    <mergeCell ref="F72:F73"/>
-    <mergeCell ref="E72:E73"/>
+    <mergeCell ref="B101:B102"/>
+    <mergeCell ref="A105:A107"/>
+    <mergeCell ref="A108:A110"/>
+    <mergeCell ref="A111:A113"/>
+    <mergeCell ref="A114:A116"/>
+    <mergeCell ref="A117:A119"/>
+    <mergeCell ref="A91:A92"/>
+    <mergeCell ref="A93:A94"/>
+    <mergeCell ref="A95:A96"/>
+    <mergeCell ref="A97:A98"/>
+    <mergeCell ref="A99:A100"/>
+    <mergeCell ref="A101:A104"/>
     <mergeCell ref="A89:A90"/>
     <mergeCell ref="A72:A74"/>
     <mergeCell ref="B72:B73"/>
@@ -3285,18 +3289,13 @@
     <mergeCell ref="A83:A84"/>
     <mergeCell ref="A85:A86"/>
     <mergeCell ref="A87:A88"/>
-    <mergeCell ref="A117:A119"/>
-    <mergeCell ref="A91:A92"/>
-    <mergeCell ref="A93:A94"/>
-    <mergeCell ref="A95:A96"/>
-    <mergeCell ref="A97:A98"/>
-    <mergeCell ref="A99:A100"/>
-    <mergeCell ref="A101:A104"/>
-    <mergeCell ref="B101:B102"/>
-    <mergeCell ref="A105:A107"/>
-    <mergeCell ref="A108:A110"/>
-    <mergeCell ref="A111:A113"/>
-    <mergeCell ref="A114:A116"/>
+    <mergeCell ref="G6:G21"/>
+    <mergeCell ref="G23:G28"/>
+    <mergeCell ref="C72:C73"/>
+    <mergeCell ref="D72:D73"/>
+    <mergeCell ref="G72:G73"/>
+    <mergeCell ref="F72:F73"/>
+    <mergeCell ref="E72:E73"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
@@ -3325,8 +3324,8 @@
     <hyperlink ref="D89" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
     <hyperlink ref="D91" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
     <hyperlink ref="D93" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="D95" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
-    <hyperlink ref="D97" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="D97" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="D95" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
     <hyperlink ref="D99" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
     <hyperlink ref="D102" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
     <hyperlink ref="D103" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
@@ -3359,17 +3358,17 @@
       <selection pane="bottomLeft" activeCell="D115" sqref="D115"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.33203125" customWidth="1"/>
-    <col min="2" max="2" width="17.6640625" customWidth="1"/>
-    <col min="3" max="3" width="63.5" customWidth="1"/>
-    <col min="4" max="4" width="72.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="57.1640625" customWidth="1"/>
+    <col min="1" max="1" width="24.28515625" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" customWidth="1"/>
+    <col min="3" max="3" width="63.42578125" customWidth="1"/>
+    <col min="4" max="4" width="72.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="57.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
@@ -3389,7 +3388,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="16">
+    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="106" t="s">
         <v>35</v>
       </c>
@@ -3404,7 +3403,7 @@
       </c>
       <c r="E2" s="8"/>
     </row>
-    <row r="3" spans="1:6" ht="16">
+    <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="106"/>
       <c r="B3" s="108"/>
       <c r="C3" s="11" t="s">
@@ -3415,7 +3414,7 @@
       </c>
       <c r="E3" s="8"/>
     </row>
-    <row r="4" spans="1:6" ht="16">
+    <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="106"/>
       <c r="B4" s="108"/>
       <c r="C4" s="11" t="s">
@@ -3426,13 +3425,13 @@
       </c>
       <c r="E4" s="11"/>
     </row>
-    <row r="5" spans="1:6" ht="16">
+    <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="106"/>
       <c r="B5" s="108"/>
       <c r="C5" s="11"/>
       <c r="E5" s="11"/>
     </row>
-    <row r="6" spans="1:6" ht="16">
+    <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="106"/>
       <c r="B6" s="108"/>
       <c r="C6" s="12" t="s">
@@ -3443,7 +3442,7 @@
       </c>
       <c r="E6" s="11"/>
     </row>
-    <row r="7" spans="1:6" ht="16">
+    <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="106"/>
       <c r="B7" s="108"/>
       <c r="C7" s="13" t="s">
@@ -3452,7 +3451,7 @@
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
     </row>
-    <row r="8" spans="1:6" ht="16">
+    <row r="8" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="106"/>
       <c r="B8" s="108"/>
       <c r="C8" s="9" t="s">
@@ -3460,7 +3459,7 @@
       </c>
       <c r="E8" s="11"/>
     </row>
-    <row r="9" spans="1:6" ht="16">
+    <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="106"/>
       <c r="B9" s="108"/>
       <c r="C9" s="9" t="s">
@@ -3469,7 +3468,7 @@
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
     </row>
-    <row r="10" spans="1:6" ht="16">
+    <row r="10" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="106"/>
       <c r="B10" s="108"/>
       <c r="C10" s="9" t="s">
@@ -3478,7 +3477,7 @@
       <c r="D10" s="11"/>
       <c r="E10" s="11"/>
     </row>
-    <row r="11" spans="1:6" ht="16">
+    <row r="11" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="106"/>
       <c r="B11" s="108"/>
       <c r="C11" s="9" t="s">
@@ -3487,7 +3486,7 @@
       <c r="D11" s="11"/>
       <c r="E11" s="11"/>
     </row>
-    <row r="12" spans="1:6" ht="16">
+    <row r="12" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="106"/>
       <c r="B12" s="108"/>
       <c r="C12" s="9" t="s">
@@ -3496,7 +3495,7 @@
       <c r="D12" s="11"/>
       <c r="E12" s="11"/>
     </row>
-    <row r="13" spans="1:6" ht="16">
+    <row r="13" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="106"/>
       <c r="B13" s="108"/>
       <c r="C13" s="9" t="s">
@@ -3505,7 +3504,7 @@
       <c r="D13" s="11"/>
       <c r="E13" s="11"/>
     </row>
-    <row r="14" spans="1:6" ht="16">
+    <row r="14" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="106"/>
       <c r="B14" s="108"/>
       <c r="C14" s="9" t="s">
@@ -3514,7 +3513,7 @@
       <c r="D14" s="11"/>
       <c r="E14" s="11"/>
     </row>
-    <row r="15" spans="1:6" ht="16">
+    <row r="15" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="106"/>
       <c r="B15" s="108"/>
       <c r="C15" s="9" t="s">
@@ -3523,7 +3522,7 @@
       <c r="D15" s="11"/>
       <c r="E15" s="11"/>
     </row>
-    <row r="16" spans="1:6" ht="16">
+    <row r="16" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="106"/>
       <c r="B16" s="108"/>
       <c r="C16" s="9" t="s">
@@ -3532,7 +3531,7 @@
       <c r="D16" s="11"/>
       <c r="E16" s="11"/>
     </row>
-    <row r="17" spans="1:6" ht="16">
+    <row r="17" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="106"/>
       <c r="B17" s="108"/>
       <c r="C17" s="9" t="s">
@@ -3541,7 +3540,7 @@
       <c r="D17" s="11"/>
       <c r="E17" s="11"/>
     </row>
-    <row r="18" spans="1:6" ht="16">
+    <row r="18" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="106"/>
       <c r="B18" s="108"/>
       <c r="C18" s="9" t="s">
@@ -3550,7 +3549,7 @@
       <c r="D18" s="11"/>
       <c r="E18" s="11"/>
     </row>
-    <row r="19" spans="1:6" ht="16">
+    <row r="19" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="106"/>
       <c r="B19" s="108"/>
       <c r="C19" s="9" t="s">
@@ -3559,7 +3558,7 @@
       <c r="D19" s="11"/>
       <c r="E19" s="11"/>
     </row>
-    <row r="20" spans="1:6" ht="16">
+    <row r="20" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="106"/>
       <c r="B20" s="108"/>
       <c r="C20" s="9" t="s">
@@ -3568,7 +3567,7 @@
       <c r="D20" s="11"/>
       <c r="E20" s="11"/>
     </row>
-    <row r="21" spans="1:6" ht="16">
+    <row r="21" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="106"/>
       <c r="B21" s="108"/>
       <c r="C21" s="10" t="s">
@@ -3577,14 +3576,14 @@
       <c r="D21" s="11"/>
       <c r="E21" s="11"/>
     </row>
-    <row r="22" spans="1:6" ht="16">
+    <row r="22" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="106"/>
       <c r="B22" s="108"/>
       <c r="C22" s="11"/>
       <c r="D22" s="11"/>
       <c r="E22" s="11"/>
     </row>
-    <row r="23" spans="1:6" ht="16">
+    <row r="23" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="106"/>
       <c r="B23" s="108"/>
       <c r="C23" s="12" t="s">
@@ -3598,7 +3597,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="16">
+    <row r="24" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="106"/>
       <c r="B24" s="108"/>
       <c r="C24" s="14" t="s">
@@ -3607,7 +3606,7 @@
       <c r="D24" s="11"/>
       <c r="E24" s="11"/>
     </row>
-    <row r="25" spans="1:6" ht="16">
+    <row r="25" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="106"/>
       <c r="B25" s="108"/>
       <c r="C25" s="15" t="s">
@@ -3615,7 +3614,7 @@
       </c>
       <c r="E25" s="11"/>
     </row>
-    <row r="26" spans="1:6" ht="16">
+    <row r="26" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="106"/>
       <c r="B26" s="108"/>
       <c r="C26" s="15" t="s">
@@ -3624,7 +3623,7 @@
       <c r="D26" s="11"/>
       <c r="E26" s="11"/>
     </row>
-    <row r="27" spans="1:6" ht="16">
+    <row r="27" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="106"/>
       <c r="B27" s="108"/>
       <c r="C27" s="15" t="s">
@@ -3633,7 +3632,7 @@
       <c r="D27" s="11"/>
       <c r="E27" s="11"/>
     </row>
-    <row r="28" spans="1:6" ht="16">
+    <row r="28" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="106"/>
       <c r="B28" s="108"/>
       <c r="C28" s="16" t="s">
@@ -3642,7 +3641,7 @@
       <c r="D28" s="11"/>
       <c r="E28" s="11"/>
     </row>
-    <row r="29" spans="1:6" ht="16">
+    <row r="29" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="106"/>
       <c r="B29" s="31" t="s">
         <v>30</v>
@@ -3652,7 +3651,7 @@
       <c r="E29" s="20"/>
       <c r="F29" s="29"/>
     </row>
-    <row r="30" spans="1:6" ht="16">
+    <row r="30" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="107"/>
       <c r="B30" s="32" t="s">
         <v>31</v>
@@ -3662,7 +3661,7 @@
       <c r="E30" s="22"/>
       <c r="F30" s="30"/>
     </row>
-    <row r="31" spans="1:6" ht="16">
+    <row r="31" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="109" t="s">
         <v>41</v>
       </c>
@@ -3672,7 +3671,7 @@
       <c r="C31" s="24"/>
       <c r="D31" s="24"/>
     </row>
-    <row r="32" spans="1:6" ht="15.5" customHeight="1">
+    <row r="32" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="110"/>
       <c r="B32" s="99"/>
       <c r="C32" s="3" t="s">
@@ -3685,7 +3684,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="16">
+    <row r="33" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="110"/>
       <c r="B33" s="99"/>
       <c r="C33" s="4" t="s">
@@ -3693,14 +3692,14 @@
       </c>
       <c r="D33" s="7"/>
     </row>
-    <row r="34" spans="1:6" ht="16">
+    <row r="34" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="110"/>
       <c r="B34" s="99"/>
       <c r="C34" s="5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="16">
+    <row r="35" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="110"/>
       <c r="B35" s="99"/>
       <c r="C35" s="5" t="s">
@@ -3708,7 +3707,7 @@
       </c>
       <c r="D35" s="7"/>
     </row>
-    <row r="36" spans="1:6" ht="16">
+    <row r="36" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="110"/>
       <c r="B36" s="99"/>
       <c r="C36" s="5" t="s">
@@ -3716,7 +3715,7 @@
       </c>
       <c r="D36" s="7"/>
     </row>
-    <row r="37" spans="1:6" ht="16">
+    <row r="37" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="110"/>
       <c r="B37" s="99"/>
       <c r="C37" s="5" t="s">
@@ -3724,7 +3723,7 @@
       </c>
       <c r="D37" s="7"/>
     </row>
-    <row r="38" spans="1:6" ht="16">
+    <row r="38" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="110"/>
       <c r="B38" s="99"/>
       <c r="C38" s="5" t="s">
@@ -3732,7 +3731,7 @@
       </c>
       <c r="D38" s="7"/>
     </row>
-    <row r="39" spans="1:6" ht="16">
+    <row r="39" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="110"/>
       <c r="B39" s="99"/>
       <c r="C39" s="5" t="s">
@@ -3740,7 +3739,7 @@
       </c>
       <c r="D39" s="7"/>
     </row>
-    <row r="40" spans="1:6" ht="16">
+    <row r="40" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="110"/>
       <c r="B40" s="99"/>
       <c r="C40" s="5" t="s">
@@ -3748,7 +3747,7 @@
       </c>
       <c r="D40" s="7"/>
     </row>
-    <row r="41" spans="1:6" ht="16">
+    <row r="41" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="110"/>
       <c r="B41" s="99"/>
       <c r="C41" s="6" t="s">
@@ -3756,7 +3755,7 @@
       </c>
       <c r="D41" s="7"/>
     </row>
-    <row r="42" spans="1:6" ht="16">
+    <row r="42" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="110"/>
       <c r="B42" s="26" t="s">
         <v>30</v>
@@ -3766,7 +3765,7 @@
       <c r="E42" s="29"/>
       <c r="F42" s="29"/>
     </row>
-    <row r="43" spans="1:6" ht="16">
+    <row r="43" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="111"/>
       <c r="B43" s="27" t="s">
         <v>31</v>
@@ -3776,7 +3775,7 @@
       <c r="E43" s="30"/>
       <c r="F43" s="30"/>
     </row>
-    <row r="44" spans="1:6">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="100" t="s">
         <v>68</v>
       </c>
@@ -3784,7 +3783,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="15.5" customHeight="1">
+    <row r="45" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="101"/>
       <c r="B45" s="99"/>
       <c r="C45" s="3" t="s">
@@ -3792,7 +3791,7 @@
       </c>
       <c r="D45" s="24"/>
     </row>
-    <row r="46" spans="1:6" ht="16">
+    <row r="46" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" s="101"/>
       <c r="B46" s="99"/>
       <c r="C46" s="5" t="s">
@@ -3805,7 +3804,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="16">
+    <row r="47" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47" s="101"/>
       <c r="B47" s="99"/>
       <c r="C47" s="5" t="s">
@@ -3815,7 +3814,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="16">
+    <row r="48" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48" s="101"/>
       <c r="B48" s="99"/>
       <c r="C48" s="5" t="s">
@@ -3826,7 +3825,7 @@
       </c>
       <c r="E48" s="7"/>
     </row>
-    <row r="49" spans="1:6" ht="16">
+    <row r="49" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A49" s="101"/>
       <c r="B49" s="99"/>
       <c r="C49" s="5" t="s">
@@ -3837,7 +3836,7 @@
       </c>
       <c r="E49" s="7"/>
     </row>
-    <row r="50" spans="1:6" ht="16">
+    <row r="50" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A50" s="101"/>
       <c r="B50" s="99"/>
       <c r="C50" s="5" t="s">
@@ -3848,7 +3847,7 @@
       </c>
       <c r="E50" s="7"/>
     </row>
-    <row r="51" spans="1:6" ht="16">
+    <row r="51" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A51" s="101"/>
       <c r="B51" s="99"/>
       <c r="C51" s="6" t="s">
@@ -3859,7 +3858,7 @@
       </c>
       <c r="E51" s="7"/>
     </row>
-    <row r="52" spans="1:6" ht="16">
+    <row r="52" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A52" s="101"/>
       <c r="B52" s="33" t="s">
         <v>30</v>
@@ -3869,7 +3868,7 @@
       <c r="E52" s="26"/>
       <c r="F52" s="29"/>
     </row>
-    <row r="53" spans="1:6" ht="16">
+    <row r="53" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A53" s="102"/>
       <c r="B53" s="34" t="s">
         <v>31</v>
@@ -3879,7 +3878,7 @@
       <c r="E53" s="27"/>
       <c r="F53" s="30"/>
     </row>
-    <row r="54" spans="1:6" ht="14.5" customHeight="1">
+    <row r="54" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="103" t="s">
         <v>69</v>
       </c>
@@ -3887,7 +3886,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="16">
+    <row r="55" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A55" s="104"/>
       <c r="B55" s="104"/>
       <c r="C55" s="3" t="s">
@@ -3896,7 +3895,7 @@
       <c r="D55" s="7"/>
       <c r="E55" s="7"/>
     </row>
-    <row r="56" spans="1:6" ht="16">
+    <row r="56" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A56" s="104"/>
       <c r="B56" s="104"/>
       <c r="C56" s="1" t="s">
@@ -3909,7 +3908,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="16">
+    <row r="57" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A57" s="104"/>
       <c r="B57" s="104"/>
       <c r="C57" s="37" t="s">
@@ -3923,7 +3922,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="58" spans="1:6" ht="16">
+    <row r="58" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A58" s="104"/>
       <c r="B58" s="104"/>
       <c r="C58" s="37" t="s">
@@ -3937,7 +3936,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="59" spans="1:6" ht="16">
+    <row r="59" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A59" s="104"/>
       <c r="B59" s="104"/>
       <c r="C59" s="37" t="s">
@@ -3951,7 +3950,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="60" spans="1:6" ht="16">
+    <row r="60" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A60" s="104"/>
       <c r="B60" s="104"/>
       <c r="C60" s="37" t="s">
@@ -3963,7 +3962,7 @@
       <c r="E60" s="7"/>
       <c r="F60" s="19"/>
     </row>
-    <row r="61" spans="1:6" ht="16">
+    <row r="61" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A61" s="104"/>
       <c r="B61" s="104"/>
       <c r="C61" s="37" t="s">
@@ -3975,7 +3974,7 @@
       <c r="E61" s="7"/>
       <c r="F61" s="19"/>
     </row>
-    <row r="62" spans="1:6" ht="16">
+    <row r="62" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A62" s="104"/>
       <c r="B62" s="104"/>
       <c r="C62" s="37" t="s">
@@ -3987,7 +3986,7 @@
       <c r="E62" s="7"/>
       <c r="F62" s="19"/>
     </row>
-    <row r="63" spans="1:6" ht="16">
+    <row r="63" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A63" s="104"/>
       <c r="B63" s="104"/>
       <c r="C63" s="37" t="s">
@@ -3999,7 +3998,7 @@
       <c r="E63" s="7"/>
       <c r="F63" s="19"/>
     </row>
-    <row r="64" spans="1:6" ht="16">
+    <row r="64" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A64" s="104"/>
       <c r="B64" s="104"/>
       <c r="C64" s="37" t="s">
@@ -4011,7 +4010,7 @@
       <c r="E64" s="7"/>
       <c r="F64" s="19"/>
     </row>
-    <row r="65" spans="1:6" ht="16">
+    <row r="65" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A65" s="104"/>
       <c r="B65" s="104"/>
       <c r="C65" s="37" t="s">
@@ -4023,7 +4022,7 @@
       <c r="E65" s="7"/>
       <c r="F65" s="19"/>
     </row>
-    <row r="66" spans="1:6" ht="16">
+    <row r="66" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A66" s="104"/>
       <c r="B66" s="104"/>
       <c r="C66" s="37" t="s">
@@ -4035,7 +4034,7 @@
       <c r="E66" s="7"/>
       <c r="F66" s="19"/>
     </row>
-    <row r="67" spans="1:6" ht="16">
+    <row r="67" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A67" s="104"/>
       <c r="B67" s="104"/>
       <c r="C67" s="5" t="s">
@@ -4049,7 +4048,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="68" spans="1:6" ht="16">
+    <row r="68" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A68" s="104"/>
       <c r="B68" s="104"/>
       <c r="C68" s="5" t="s">
@@ -4061,7 +4060,7 @@
       <c r="E68" s="7"/>
       <c r="F68" s="19"/>
     </row>
-    <row r="69" spans="1:6" ht="16">
+    <row r="69" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A69" s="104"/>
       <c r="B69" s="104"/>
       <c r="C69" s="5" t="s">
@@ -4073,7 +4072,7 @@
       <c r="E69" s="7"/>
       <c r="F69" s="19"/>
     </row>
-    <row r="70" spans="1:6" ht="32">
+    <row r="70" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A70" s="104"/>
       <c r="B70" s="104"/>
       <c r="C70" s="6" t="s">
@@ -4087,7 +4086,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="71" spans="1:6" ht="16">
+    <row r="71" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A71" s="105"/>
       <c r="B71" s="27" t="s">
         <v>108</v>
@@ -4097,11 +4096,11 @@
       <c r="E71" s="30"/>
       <c r="F71" s="30"/>
     </row>
-    <row r="72" spans="1:6" ht="16">
-      <c r="A72" s="83" t="s">
+    <row r="72" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A72" s="84" t="s">
         <v>109</v>
       </c>
-      <c r="B72" s="91" t="s">
+      <c r="B72" s="80" t="s">
         <v>70</v>
       </c>
       <c r="C72" s="24"/>
@@ -4109,9 +4108,9 @@
       <c r="E72" s="24"/>
       <c r="F72" s="24"/>
     </row>
-    <row r="73" spans="1:6" ht="16">
-      <c r="A73" s="90"/>
-      <c r="B73" s="92"/>
+    <row r="73" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A73" s="86"/>
+      <c r="B73" s="81"/>
       <c r="C73" s="7" t="s">
         <v>110</v>
       </c>
@@ -4122,8 +4121,8 @@
         <v>136</v>
       </c>
     </row>
-    <row r="74" spans="1:6" ht="16">
-      <c r="A74" s="84"/>
+    <row r="74" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A74" s="85"/>
       <c r="B74" s="27" t="s">
         <v>111</v>
       </c>
@@ -4132,8 +4131,8 @@
       <c r="E74" s="23"/>
       <c r="F74" s="23"/>
     </row>
-    <row r="75" spans="1:6" ht="16">
-      <c r="A75" s="83" t="s">
+    <row r="75" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A75" s="84" t="s">
         <v>73</v>
       </c>
       <c r="B75" s="24" t="s">
@@ -4149,8 +4148,8 @@
         <v>136</v>
       </c>
     </row>
-    <row r="76" spans="1:6" ht="16">
-      <c r="A76" s="84"/>
+    <row r="76" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A76" s="85"/>
       <c r="B76" s="27" t="s">
         <v>111</v>
       </c>
@@ -4159,8 +4158,8 @@
       <c r="E76" s="23"/>
       <c r="F76" s="23"/>
     </row>
-    <row r="77" spans="1:6" ht="16">
-      <c r="A77" s="83" t="s">
+    <row r="77" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A77" s="84" t="s">
         <v>75</v>
       </c>
       <c r="B77" s="24" t="s">
@@ -4177,8 +4176,8 @@
         <v>136</v>
       </c>
     </row>
-    <row r="78" spans="1:6" ht="16">
-      <c r="A78" s="84"/>
+    <row r="78" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A78" s="85"/>
       <c r="B78" s="27" t="s">
         <v>111</v>
       </c>
@@ -4187,8 +4186,8 @@
       <c r="E78" s="23"/>
       <c r="F78" s="23"/>
     </row>
-    <row r="79" spans="1:6" ht="16">
-      <c r="A79" s="83" t="s">
+    <row r="79" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A79" s="84" t="s">
         <v>77</v>
       </c>
       <c r="B79" s="24" t="s">
@@ -4205,8 +4204,8 @@
         <v>136</v>
       </c>
     </row>
-    <row r="80" spans="1:6" ht="16">
-      <c r="A80" s="84"/>
+    <row r="80" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A80" s="85"/>
       <c r="B80" s="27" t="s">
         <v>111</v>
       </c>
@@ -4215,8 +4214,8 @@
       <c r="E80" s="23"/>
       <c r="F80" s="23"/>
     </row>
-    <row r="81" spans="1:6" ht="16">
-      <c r="A81" s="83" t="s">
+    <row r="81" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A81" s="84" t="s">
         <v>79</v>
       </c>
       <c r="B81" s="24" t="s">
@@ -4233,8 +4232,8 @@
         <v>136</v>
       </c>
     </row>
-    <row r="82" spans="1:6" ht="16">
-      <c r="A82" s="84"/>
+    <row r="82" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A82" s="85"/>
       <c r="B82" s="27" t="s">
         <v>111</v>
       </c>
@@ -4243,8 +4242,8 @@
       <c r="E82" s="23"/>
       <c r="F82" s="23"/>
     </row>
-    <row r="83" spans="1:6" ht="16">
-      <c r="A83" s="83" t="s">
+    <row r="83" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A83" s="84" t="s">
         <v>81</v>
       </c>
       <c r="B83" s="24" t="s">
@@ -4261,8 +4260,8 @@
         <v>136</v>
       </c>
     </row>
-    <row r="84" spans="1:6" ht="16">
-      <c r="A84" s="84"/>
+    <row r="84" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A84" s="85"/>
       <c r="B84" s="27" t="s">
         <v>111</v>
       </c>
@@ -4271,8 +4270,8 @@
       <c r="E84" s="23"/>
       <c r="F84" s="23"/>
     </row>
-    <row r="85" spans="1:6" ht="16">
-      <c r="A85" s="83" t="s">
+    <row r="85" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A85" s="84" t="s">
         <v>83</v>
       </c>
       <c r="B85" s="24" t="s">
@@ -4289,8 +4288,8 @@
         <v>136</v>
       </c>
     </row>
-    <row r="86" spans="1:6" ht="16">
-      <c r="A86" s="84"/>
+    <row r="86" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A86" s="85"/>
       <c r="B86" s="27" t="s">
         <v>111</v>
       </c>
@@ -4299,8 +4298,8 @@
       <c r="E86" s="23"/>
       <c r="F86" s="23"/>
     </row>
-    <row r="87" spans="1:6" ht="16">
-      <c r="A87" s="83" t="s">
+    <row r="87" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A87" s="84" t="s">
         <v>85</v>
       </c>
       <c r="B87" s="24" t="s">
@@ -4317,8 +4316,8 @@
         <v>136</v>
       </c>
     </row>
-    <row r="88" spans="1:6" ht="16">
-      <c r="A88" s="84"/>
+    <row r="88" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A88" s="85"/>
       <c r="B88" s="27" t="s">
         <v>111</v>
       </c>
@@ -4327,8 +4326,8 @@
       <c r="E88" s="23"/>
       <c r="F88" s="23"/>
     </row>
-    <row r="89" spans="1:6" ht="16">
-      <c r="A89" s="83" t="s">
+    <row r="89" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A89" s="84" t="s">
         <v>87</v>
       </c>
       <c r="B89" s="24" t="s">
@@ -4345,8 +4344,8 @@
         <v>136</v>
       </c>
     </row>
-    <row r="90" spans="1:6" ht="16">
-      <c r="A90" s="84"/>
+    <row r="90" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A90" s="85"/>
       <c r="B90" s="27" t="s">
         <v>111</v>
       </c>
@@ -4355,8 +4354,8 @@
       <c r="E90" s="23"/>
       <c r="F90" s="23"/>
     </row>
-    <row r="91" spans="1:6" ht="16">
-      <c r="A91" s="83" t="s">
+    <row r="91" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A91" s="84" t="s">
         <v>89</v>
       </c>
       <c r="B91" s="24" t="s">
@@ -4373,8 +4372,8 @@
         <v>136</v>
       </c>
     </row>
-    <row r="92" spans="1:6" ht="16">
-      <c r="A92" s="84"/>
+    <row r="92" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A92" s="85"/>
       <c r="B92" s="27" t="s">
         <v>111</v>
       </c>
@@ -4383,8 +4382,8 @@
       <c r="E92" s="23"/>
       <c r="F92" s="23"/>
     </row>
-    <row r="93" spans="1:6" ht="16">
-      <c r="A93" s="83" t="s">
+    <row r="93" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A93" s="84" t="s">
         <v>91</v>
       </c>
       <c r="B93" s="24" t="s">
@@ -4401,8 +4400,8 @@
         <v>136</v>
       </c>
     </row>
-    <row r="94" spans="1:6" ht="16">
-      <c r="A94" s="84"/>
+    <row r="94" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A94" s="85"/>
       <c r="B94" s="27" t="s">
         <v>111</v>
       </c>
@@ -4411,8 +4410,8 @@
       <c r="E94" s="23"/>
       <c r="F94" s="23"/>
     </row>
-    <row r="95" spans="1:6" ht="16">
-      <c r="A95" s="85" t="s">
+    <row r="95" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A95" s="90" t="s">
         <v>112</v>
       </c>
       <c r="B95" s="24" t="s">
@@ -4429,8 +4428,8 @@
         <v>136</v>
       </c>
     </row>
-    <row r="96" spans="1:6" ht="16">
-      <c r="A96" s="84"/>
+    <row r="96" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A96" s="85"/>
       <c r="B96" s="27" t="s">
         <v>111</v>
       </c>
@@ -4439,8 +4438,8 @@
       <c r="E96" s="23"/>
       <c r="F96" s="23"/>
     </row>
-    <row r="97" spans="1:6" ht="16">
-      <c r="A97" s="86" t="s">
+    <row r="97" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A97" s="91" t="s">
         <v>113</v>
       </c>
       <c r="B97" s="24" t="s">
@@ -4457,8 +4456,8 @@
         <v>136</v>
       </c>
     </row>
-    <row r="98" spans="1:6" ht="16">
-      <c r="A98" s="79"/>
+    <row r="98" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A98" s="92"/>
       <c r="B98" s="27" t="s">
         <v>111</v>
       </c>
@@ -4467,8 +4466,8 @@
       <c r="E98" s="23"/>
       <c r="F98" s="23"/>
     </row>
-    <row r="99" spans="1:6" ht="16">
-      <c r="A99" s="83" t="s">
+    <row r="99" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A99" s="84" t="s">
         <v>114</v>
       </c>
       <c r="B99" s="24" t="s">
@@ -4485,8 +4484,8 @@
         <v>136</v>
       </c>
     </row>
-    <row r="100" spans="1:6" ht="16">
-      <c r="A100" s="84"/>
+    <row r="100" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A100" s="85"/>
       <c r="B100" s="27" t="s">
         <v>111</v>
       </c>
@@ -4495,20 +4494,20 @@
       <c r="E100" s="23"/>
       <c r="F100" s="23"/>
     </row>
-    <row r="101" spans="1:6" ht="16">
-      <c r="A101" s="87" t="s">
+    <row r="101" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A101" s="93" t="s">
         <v>115</v>
       </c>
-      <c r="B101" s="75" t="s">
+      <c r="B101" s="76" t="s">
         <v>70</v>
       </c>
       <c r="C101" s="7"/>
       <c r="D101" s="7"/>
       <c r="F101" s="35"/>
     </row>
-    <row r="102" spans="1:6" ht="16">
-      <c r="A102" s="88"/>
-      <c r="B102" s="76"/>
+    <row r="102" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A102" s="94"/>
+      <c r="B102" s="77"/>
       <c r="C102" s="7" t="s">
         <v>116</v>
       </c>
@@ -4519,8 +4518,8 @@
         <v>156</v>
       </c>
     </row>
-    <row r="103" spans="1:6" ht="16">
-      <c r="A103" s="88"/>
+    <row r="103" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A103" s="94"/>
       <c r="B103" s="7" t="s">
         <v>118</v>
       </c>
@@ -4534,8 +4533,8 @@
         <v>157</v>
       </c>
     </row>
-    <row r="104" spans="1:6" ht="16">
-      <c r="A104" s="88"/>
+    <row r="104" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A104" s="94"/>
       <c r="B104" s="26" t="s">
         <v>31</v>
       </c>
@@ -4543,8 +4542,8 @@
       <c r="D104" s="7"/>
       <c r="F104" s="35"/>
     </row>
-    <row r="105" spans="1:6" ht="16">
-      <c r="A105" s="78" t="s">
+    <row r="105" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A105" s="97" t="s">
         <v>121</v>
       </c>
       <c r="B105" s="39" t="s">
@@ -4560,8 +4559,8 @@
         <v>159</v>
       </c>
     </row>
-    <row r="106" spans="1:6" ht="16">
-      <c r="A106" s="78"/>
+    <row r="106" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A106" s="97"/>
       <c r="B106" s="39" t="s">
         <v>118</v>
       </c>
@@ -4575,8 +4574,8 @@
         <v>158</v>
       </c>
     </row>
-    <row r="107" spans="1:6" ht="16">
-      <c r="A107" s="78"/>
+    <row r="107" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A107" s="97"/>
       <c r="B107" s="46" t="s">
         <v>31</v>
       </c>
@@ -4584,8 +4583,8 @@
       <c r="D107" s="7"/>
       <c r="F107" s="50"/>
     </row>
-    <row r="108" spans="1:6" ht="16">
-      <c r="A108" s="78" t="s">
+    <row r="108" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A108" s="97" t="s">
         <v>124</v>
       </c>
       <c r="B108" s="39" t="s">
@@ -4599,8 +4598,8 @@
       </c>
       <c r="F108" s="35"/>
     </row>
-    <row r="109" spans="1:6" ht="16">
-      <c r="A109" s="78"/>
+    <row r="109" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A109" s="97"/>
       <c r="B109" s="39" t="s">
         <v>118</v>
       </c>
@@ -4614,8 +4613,8 @@
         <v>160</v>
       </c>
     </row>
-    <row r="110" spans="1:6" ht="16">
-      <c r="A110" s="78"/>
+    <row r="110" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A110" s="97"/>
       <c r="B110" s="46" t="s">
         <v>31</v>
       </c>
@@ -4623,8 +4622,8 @@
       <c r="D110" s="7"/>
       <c r="F110" s="35"/>
     </row>
-    <row r="111" spans="1:6" ht="16">
-      <c r="A111" s="78" t="s">
+    <row r="111" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A111" s="97" t="s">
         <v>127</v>
       </c>
       <c r="B111" s="39" t="s">
@@ -4638,8 +4637,8 @@
       </c>
       <c r="F111" s="35"/>
     </row>
-    <row r="112" spans="1:6" ht="16">
-      <c r="A112" s="78"/>
+    <row r="112" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A112" s="97"/>
       <c r="B112" s="39" t="s">
         <v>118</v>
       </c>
@@ -4653,8 +4652,8 @@
         <v>161</v>
       </c>
     </row>
-    <row r="113" spans="1:6" ht="16">
-      <c r="A113" s="78"/>
+    <row r="113" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A113" s="97"/>
       <c r="B113" s="46" t="s">
         <v>31</v>
       </c>
@@ -4662,8 +4661,8 @@
       <c r="D113" s="7"/>
       <c r="F113" s="35"/>
     </row>
-    <row r="114" spans="1:6" ht="16">
-      <c r="A114" s="78" t="s">
+    <row r="114" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A114" s="97" t="s">
         <v>130</v>
       </c>
       <c r="B114" s="39" t="s">
@@ -4677,8 +4676,8 @@
       </c>
       <c r="F114" s="35"/>
     </row>
-    <row r="115" spans="1:6" ht="16">
-      <c r="A115" s="78"/>
+    <row r="115" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A115" s="97"/>
       <c r="B115" s="39" t="s">
         <v>118</v>
       </c>
@@ -4692,8 +4691,8 @@
         <v>162</v>
       </c>
     </row>
-    <row r="116" spans="1:6" ht="16">
-      <c r="A116" s="78"/>
+    <row r="116" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A116" s="97"/>
       <c r="B116" s="46" t="s">
         <v>31</v>
       </c>
@@ -4701,8 +4700,8 @@
       <c r="D116" s="7"/>
       <c r="F116" s="35"/>
     </row>
-    <row r="117" spans="1:6" ht="16">
-      <c r="A117" s="81" t="s">
+    <row r="117" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A117" s="88" t="s">
         <v>133</v>
       </c>
       <c r="B117" s="39" t="s">
@@ -4716,8 +4715,8 @@
       </c>
       <c r="F117" s="35"/>
     </row>
-    <row r="118" spans="1:6" ht="16">
-      <c r="A118" s="81"/>
+    <row r="118" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A118" s="88"/>
       <c r="B118" s="39" t="s">
         <v>118</v>
       </c>
@@ -4731,8 +4730,8 @@
         <v>163</v>
       </c>
     </row>
-    <row r="119" spans="1:6" ht="16">
-      <c r="A119" s="82"/>
+    <row r="119" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A119" s="89"/>
       <c r="B119" s="49" t="s">
         <v>31</v>
       </c>
@@ -4741,7 +4740,7 @@
       <c r="E119" s="23"/>
       <c r="F119" s="51"/>
     </row>
-    <row r="120" spans="1:6" ht="16">
+    <row r="120" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A120" s="45" t="s">
         <v>137</v>
       </c>
@@ -4749,7 +4748,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="121" spans="1:6" ht="16">
+    <row r="121" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A121" s="45" t="s">
         <v>138</v>
       </c>
@@ -4757,7 +4756,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="122" spans="1:6" ht="16">
+    <row r="122" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A122" s="45" t="s">
         <v>139</v>
       </c>
@@ -4765,7 +4764,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="123" spans="1:6" ht="16">
+    <row r="123" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A123" s="47" t="s">
         <v>140</v>
       </c>
@@ -4773,7 +4772,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="124" spans="1:6" ht="16">
+    <row r="124" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A124" s="47" t="s">
         <v>141</v>
       </c>
@@ -4781,7 +4780,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="125" spans="1:6" ht="16">
+    <row r="125" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A125" s="47" t="s">
         <v>142</v>
       </c>
@@ -4789,7 +4788,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="126" spans="1:6" ht="16">
+    <row r="126" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A126" s="47" t="s">
         <v>143</v>
       </c>
@@ -4797,7 +4796,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="127" spans="1:6" ht="16">
+    <row r="127" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A127" s="47" t="s">
         <v>144</v>
       </c>
@@ -4805,7 +4804,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="128" spans="1:6" ht="16">
+    <row r="128" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A128" s="47" t="s">
         <v>145</v>
       </c>
@@ -4813,7 +4812,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="129" spans="1:6" ht="16">
+    <row r="129" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A129" s="47" t="s">
         <v>146</v>
       </c>
@@ -4821,7 +4820,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="130" spans="1:6" ht="16">
+    <row r="130" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A130" s="47" t="s">
         <v>147</v>
       </c>
@@ -4829,7 +4828,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="131" spans="1:6" ht="16">
+    <row r="131" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A131" s="47" t="s">
         <v>148</v>
       </c>
@@ -4837,7 +4836,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="132" spans="1:6" ht="16">
+    <row r="132" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A132" s="47" t="s">
         <v>149</v>
       </c>
@@ -4845,7 +4844,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="133" spans="1:6" ht="16">
+    <row r="133" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A133" s="47" t="s">
         <v>150</v>
       </c>
@@ -4853,7 +4852,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="134" spans="1:6" ht="16">
+    <row r="134" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A134" s="47" t="s">
         <v>151</v>
       </c>
@@ -4861,7 +4860,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="135" spans="1:6" ht="16">
+    <row r="135" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A135" s="47" t="s">
         <v>152</v>
       </c>
@@ -4869,7 +4868,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="136" spans="1:6" ht="16">
+    <row r="136" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A136" s="47" t="s">
         <v>153</v>
       </c>
@@ -4877,7 +4876,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="137" spans="1:6" ht="16">
+    <row r="137" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A137" s="47" t="s">
         <v>154</v>
       </c>
@@ -4885,7 +4884,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="138" spans="1:6" ht="16">
+    <row r="138" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A138" s="48" t="s">
         <v>155</v>
       </c>
@@ -4899,14 +4898,12 @@
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="B44:B51"/>
-    <mergeCell ref="A44:A53"/>
-    <mergeCell ref="B54:B70"/>
-    <mergeCell ref="A54:A71"/>
-    <mergeCell ref="A2:A30"/>
-    <mergeCell ref="B2:B28"/>
-    <mergeCell ref="A31:A43"/>
-    <mergeCell ref="B31:B41"/>
+    <mergeCell ref="A108:A110"/>
+    <mergeCell ref="A111:A113"/>
+    <mergeCell ref="A114:A116"/>
+    <mergeCell ref="A117:A119"/>
+    <mergeCell ref="B101:B102"/>
+    <mergeCell ref="A105:A107"/>
     <mergeCell ref="A97:A98"/>
     <mergeCell ref="A99:A100"/>
     <mergeCell ref="A72:A74"/>
@@ -4923,12 +4920,14 @@
     <mergeCell ref="A79:A80"/>
     <mergeCell ref="A81:A82"/>
     <mergeCell ref="A83:A84"/>
-    <mergeCell ref="A108:A110"/>
-    <mergeCell ref="A111:A113"/>
-    <mergeCell ref="A114:A116"/>
-    <mergeCell ref="A117:A119"/>
-    <mergeCell ref="B101:B102"/>
-    <mergeCell ref="A105:A107"/>
+    <mergeCell ref="B44:B51"/>
+    <mergeCell ref="A44:A53"/>
+    <mergeCell ref="B54:B70"/>
+    <mergeCell ref="A54:A71"/>
+    <mergeCell ref="A2:A30"/>
+    <mergeCell ref="B2:B28"/>
+    <mergeCell ref="A31:A43"/>
+    <mergeCell ref="B31:B41"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>

</xml_diff>